<commit_message>
Major framework optimization and enhancements (Dec 4, 2025)
- PO Files: Standardized patterns, ThreadLocal variables, removed IOException from constructors
- BasePageObject: Added centralized locators, checkbox counting helpers, date formatting
- Duplicate logs removed from PO21
- Profile counting: Added 3 categories (Selected/Unselected/Disabled) with JavaScript for performance
- Scroll logging: Added verbose progress logs for long scroll operations
- Cross-browser runners: Simplified with new CrossBrowserCucumberRunner base class
- DailyExcelTracker: Reduced INFO logging by ~62%
- log4j2.properties: Optimized configuration, removed redundant appenders
- Deleted unused files: HeadlessCompatibleActions.java, extent.properties
- Moved PageObjectHelper to utils/JobMapping package
- Fixed success popup verification timeout in PO04
- Enabled publish success popup verification in feature file
</commit_message>
<xml_diff>
--- a/e2e-automation/src/test/resources/testdata/TestData.xlsx
+++ b/e2e-automation/src/test/resources/testdata/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Job Mapping\e2e-automation\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{791BE651-1AF5-44CA-8B8F-DE51C09D758B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14EDBDF8-1B22-4342-B863-086995C765E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -475,7 +475,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -543,7 +543,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>14</v>
@@ -595,7 +595,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>23</v>

</xml_diff>

<commit_message>
Replace Extent Reports with Allure Reporting integration
- Removed all Extent Reports references from codebase
- Updated GitHub Actions workflow to use Allure Reports
- Added Allure reporting flag in config.properties
- Integrated Allure screenshot attachments and environment info
- Updated all 87 test runners with Allure integration
- Updated README.md documentation
- Added AllureScreenshotListener, AllureEnvironmentInfo, and DailyAllureManager utilities
</commit_message>
<xml_diff>
--- a/e2e-automation/src/test/resources/testdata/TestData.xlsx
+++ b/e2e-automation/src/test/resources/testdata/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Job Mapping\e2e-automation\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14EDBDF8-1B22-4342-B863-086995C765E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ED681B2-755D-4903-9FEC-53F84DD8B0DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -475,7 +475,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -543,7 +543,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>14</v>
@@ -595,7 +595,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>23</v>

</xml_diff>

<commit_message>
Fix parallel execution issues and improve CI/CD workflow - Convert static variables to ThreadLocal in PO11 for thread safety - Fix stale element references in filter validation methods - Add job name verification in published job validation methods - Fix username retrieval in Excel reports (prioritize PO01_KFoneLogin) - Add CI/CD override support for Login Type and PAMS ID - Simplify YAML workflow file - Improve Allure report generation with better error handling
</commit_message>
<xml_diff>
--- a/e2e-automation/src/test/resources/testdata/TestData.xlsx
+++ b/e2e-automation/src/test/resources/testdata/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Job Mapping\e2e-automation\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ED681B2-755D-4903-9FEC-53F84DD8B0DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7251F39-F4EB-4D96-B284-7406EAC10709}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -475,7 +475,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Fix TimeoutException - Chrome memory optimization + thread reduction
CHROME STABILITY FIXES (DriverManager.java):
- Added --memory-pressure-off to prevent memory-related timeouts
- Added --max-old-space-size=4096 for better JS heap management
- Added --disable-features=VizDisplayCompositor for stability
- Added --single-process to reduce memory footprint in headless mode
- Set PageLoadStrategy.NORMAL explicitly

THREAD COUNT (JAM_SanityTestSuite.xml):
- Reduced from 4 to 3 threads for better stability

Root Cause: Multiple parallel browser instances competing for memory/CPU
caused java.util.concurrent.TimeoutException
</commit_message>
<xml_diff>
--- a/e2e-automation/src/test/resources/testdata/TestData.xlsx
+++ b/e2e-automation/src/test/resources/testdata/TestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Job Mapping\e2e-automation\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7251F39-F4EB-4D96-B284-7406EAC10709}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBE0008F-D9F2-4C87-B942-8E0ACA92DAA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4740" yWindow="312" windowWidth="15096" windowHeight="11928" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginData" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="30">
   <si>
     <t>TestID</t>
   </si>
@@ -113,6 +113,9 @@
   </si>
   <si>
     <t>Environment</t>
+  </si>
+  <si>
+    <t>202512KFLog!</t>
   </si>
 </sst>
 </file>
@@ -475,7 +478,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -636,7 +639,7 @@
         <v>9</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="G6" s="2">
         <v>12024</v>

</xml_diff>